<commit_message>
Actualizacion del repositorio modelo entidad relacion y organizacion de las carpetas
</commit_message>
<xml_diff>
--- a/Documentos Sprint/ProducBacklogDIVI.xlsx
+++ b/Documentos Sprint/ProducBacklogDIVI.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maycol\Desktop\MisionTic\Ciclo 3\Sprint 1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maycol\Documents\Coding\MisionTic Ciclo 3\ProjectDivi\ProyectoCiclo3Alquiler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D77EF5AD-1743-4223-B483-6131237FCD68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43CBF5-B84F-4ED1-8A95-13436776A950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1765,7 +1765,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1862,10 +1862,10 @@
         <v>44439</v>
       </c>
       <c r="D6" s="22">
-        <v>44479</v>
+        <v>44449</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1899,7 +1899,7 @@
         <v>44443</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1933,7 +1933,7 @@
         <v>44444</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1970,7 +1970,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2016,10 +2016,10 @@
         <v>44445</v>
       </c>
       <c r="D3" s="22">
-        <v>44452</v>
+        <v>44457</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2033,10 +2033,10 @@
         <v>44445</v>
       </c>
       <c r="D4" s="22">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2050,10 +2050,10 @@
         <v>44445</v>
       </c>
       <c r="D5" s="22">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2067,10 +2067,10 @@
         <v>44445</v>
       </c>
       <c r="D6" s="22">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2084,10 +2084,10 @@
         <v>44445</v>
       </c>
       <c r="D7" s="22">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,16 +2095,16 @@
         <v>17</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C8" s="22">
         <v>44445</v>
       </c>
       <c r="D8" s="22">
-        <v>44450</v>
+        <v>44457</v>
       </c>
       <c r="E8" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion documento definicion del proyecto y alcance
</commit_message>
<xml_diff>
--- a/Documentos Sprint/ProducBacklogDIVI.xlsx
+++ b/Documentos Sprint/ProducBacklogDIVI.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maycol\Documents\Coding\MisionTic Ciclo 3\ProjectDivi\ProyectoCiclo3Alquiler\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIZABETH GUANCHA\Documents\Diplomado Tic 2022\Ciclo tres\ProyectoCiclo3Alquiler\Documentos Sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA43CBF5-B84F-4ED1-8A95-13436776A950}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -224,7 +223,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -614,7 +613,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -686,7 +684,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -758,7 +755,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -822,7 +818,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -886,7 +881,6 @@
         <sz val="12"/>
         <color theme="1"/>
         <name val="Calibri"/>
-        <family val="2"/>
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -1007,17 +1001,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{45713D15-D563-4FF5-BCDD-9AFFA706C57C}">
+    <tableStyle name="Table Style 1" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="51"/>
       <tableStyleElement type="firstRowStripe" dxfId="50"/>
       <tableStyleElement type="secondRowStripe" dxfId="49"/>
     </tableStyle>
-    <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{0AE62D85-4BF3-400E-B0A7-FBEFB73B7199}">
+    <tableStyle name="Table Style 2" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="48"/>
       <tableStyleElement type="firstRowStripe" dxfId="47"/>
       <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
-    <tableStyle name="Table Style 3" pivot="0" count="3" xr9:uid="{CC58DBC0-0143-4ECE-86BA-208F7820B923}">
+    <tableStyle name="Table Style 3" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
       <tableStyleElement type="secondRowStripe" dxfId="43"/>
@@ -1049,70 +1043,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D836CC97-3F25-4FDD-B952-B3808D4002A9}" name="Table1" displayName="Table1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="39">
-  <autoFilter ref="A2:E10" xr:uid="{D836CC97-3F25-4FDD-B952-B3808D4002A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="39">
+  <autoFilter ref="A2:E10"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{DD5B40F6-A916-4606-B6C9-6DC1B572761C}" name="TAREA"/>
-    <tableColumn id="2" xr3:uid="{DEBDFFE1-BB68-4454-AA18-9172C7CB1AE8}" name="RESPONSABLE" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{A98E0CC4-D09C-47C5-8FEC-DD9521C8270A}" name="FECHA INICIO" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{C72275BC-4983-46C7-9B93-9620C97A28D4}" name="FECHA FIN" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{C0F7AD90-53F1-4FC7-9866-2E581EA79B03}" name="ESTADO" dataDxfId="35"/>
+    <tableColumn id="1" name="TAREA"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="38"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="37"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="36"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C69AE6C8-07C6-4E3F-81FC-51D6C156B67A}" name="Table13" displayName="Table13" ref="A2:E8" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A2:E8" xr:uid="{D836CC97-3F25-4FDD-B952-B3808D4002A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:E8" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A2:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{80D20BE9-6FEE-4A4D-BA56-4F38420FBCE2}" name="TAREA"/>
-    <tableColumn id="2" xr3:uid="{301F0F40-6134-4164-8FAA-9090CC2C6209}" name="RESPONSABLE" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{E8B13680-0D80-4C0D-8398-7D73BEE3D5DF}" name="FECHA INICIO" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{E3F765D4-2BDF-46BA-AE1A-AAF6D7D3ABE6}" name="FECHA FIN" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{F2E2B3C3-F3F7-49A5-B323-D983F28D5E00}" name="ESTADO" dataDxfId="27"/>
+    <tableColumn id="1" name="TAREA"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="30"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="29"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="28"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{088EEB15-D783-462A-977A-63CFE42A600A}" name="Table134" displayName="Table134" ref="A2:E8" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A2:E8" xr:uid="{D836CC97-3F25-4FDD-B952-B3808D4002A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A2:E8" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A2:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{B0383C04-A9D2-4C07-A16F-DB2D24F166A9}" name="TAREA" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{E918514E-4085-443C-9092-50EA84EF4596}" name="RESPONSABLE" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{563DB8AD-BA37-4AF6-B9FB-FC4444E16F89}" name="FECHA INICIO" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{8A6F2C05-EC3A-4863-B372-F82240653CBB}" name="FECHA FIN" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{5A4B2233-6C91-4B2A-9766-9B57438C0C74}" name="ESTADO" dataDxfId="18"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="22"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="21"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="20"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="19"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{B445DA11-1A5C-42F9-A59C-BC5EED24CB1A}" name="Table1345" displayName="Table1345" ref="A2:E11" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A2:E11" xr:uid="{D836CC97-3F25-4FDD-B952-B3808D4002A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A2:E11" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A2:E11"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{FE0D1B0D-36E8-418C-9DE6-B56DD376E178}" name="TAREA" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{BB49E75F-10F1-4BEC-84CE-D85F1EFFC040}" name="RESPONSABLE" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00913A7E-F1F4-40FC-B843-E1AF242F0D5F}" name="FECHA INICIO" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{5E7B683A-E09D-4B95-9AEF-F18B8877B9FE}" name="FECHA FIN" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{BF2B589D-D6BF-4D52-972E-A4FD45F9E48B}" name="ESTADO" dataDxfId="9"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="13"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="12"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="11"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="10"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{60A14CF9-B2DB-47F4-BFFD-B1F1C0EDF577}" name="Table13456" displayName="Table13456" ref="A2:E9" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A2:E9" xr:uid="{D836CC97-3F25-4FDD-B952-B3808D4002A9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A2:E9" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A2:E9"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{572BAF1A-7DCE-4A54-91F3-6ED0ED6DD23E}" name="TAREA" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{AF71381A-E14E-48F4-9E21-07607D9F805A}" name="RESPONSABLE" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{4C9D297F-1E30-4A12-8C0A-3475259094FA}" name="FECHA INICIO" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{35323700-4A26-4DF3-9A57-E73751D8E584}" name="FECHA FIN" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{12B36C55-E2F7-476B-BB3F-A9FEC39D57E0}" name="ESTADO" dataDxfId="0"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="4"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="3"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="2"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="1"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1380,14 +1374,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32:B38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
@@ -1761,14 +1755,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C21E0CB-6134-4B09-8469-ECF1FB101D46}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
@@ -1916,7 +1910,7 @@
         <v>44443</v>
       </c>
       <c r="E9" s="15" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1954,7 +1948,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10" xr:uid="{772D2774-56DE-47A0-A41E-9364CCE2E14C}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1966,14 +1960,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BE24296-9BC8-4A11-93B8-16D5FE0728FB}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
@@ -2019,7 +2013,7 @@
         <v>44457</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2125,7 +2119,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8" xr:uid="{0AFFDA34-389F-45C8-8F8B-F7BB578A8192}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2137,14 +2131,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D15FED3-1473-48BF-B0F5-C3AE053DA4FD}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
@@ -2296,7 +2290,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8" xr:uid="{89316B98-58AE-4CA3-AF5B-0E546BD062D7}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2308,14 +2302,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42E207DD-CDC7-407C-B6B3-BFB3C32075D4}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="96.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
@@ -2518,7 +2512,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E11" xr:uid="{CD3BE814-7FD4-4233-BCF4-5C76A5545221}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E11">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2530,14 +2524,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D4FF1F0A-A305-48E7-B3BD-C02823EB40A9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="96.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="5" width="20.7109375" customWidth="1"/>
@@ -2706,7 +2700,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E9" xr:uid="{7397E314-0859-4395-BA8F-5B75231030C9}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E9">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Actualizacion cabios finales base de datos, diagrama entidad relacion, finalizacion formulario usuario inicio login
</commit_message>
<xml_diff>
--- a/Documentos Sprint/ProducBacklogDIVI.xlsx
+++ b/Documentos Sprint/ProducBacklogDIVI.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Curso Programacion\Programacion\Ciclo 3\Proyecto Ciclo 3\ProyectoCiclo3Alquiler\Documentos Sprint\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ELIZABETH GUANCHA\Documents\Diplomado Tic 2022\Ciclo tres\ProyectoCiclo3Alquiler\Documentos Sprint\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A80A11-F65D-4793-908C-B1DF681A57DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -224,7 +223,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1002,17 +1001,17 @@
     </dxf>
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
-    <tableStyle name="Table Style 1" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
+    <tableStyle name="Table Style 1" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="51"/>
       <tableStyleElement type="firstRowStripe" dxfId="50"/>
       <tableStyleElement type="secondRowStripe" dxfId="49"/>
     </tableStyle>
-    <tableStyle name="Table Style 2" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF01000000}">
+    <tableStyle name="Table Style 2" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="48"/>
       <tableStyleElement type="firstRowStripe" dxfId="47"/>
       <tableStyleElement type="secondRowStripe" dxfId="46"/>
     </tableStyle>
-    <tableStyle name="Table Style 3" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF02000000}">
+    <tableStyle name="Table Style 3" pivot="0" count="3">
       <tableStyleElement type="headerRow" dxfId="45"/>
       <tableStyleElement type="firstRowStripe" dxfId="44"/>
       <tableStyleElement type="secondRowStripe" dxfId="43"/>
@@ -1044,70 +1043,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="39">
-  <autoFilter ref="A2:E10" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="39">
+  <autoFilter ref="A2:E10"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="TAREA"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="RESPONSABLE" dataDxfId="38"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="FECHA INICIO" dataDxfId="37"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="FECHA FIN" dataDxfId="36"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="ESTADO" dataDxfId="35"/>
+    <tableColumn id="1" name="TAREA"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="38"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="37"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="36"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Table13" displayName="Table13" ref="A2:E8" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A2:E8" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:E8" totalsRowShown="0" headerRowDxfId="31">
+  <autoFilter ref="A2:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="TAREA"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0100-000002000000}" name="RESPONSABLE" dataDxfId="30"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="FECHA INICIO" dataDxfId="29"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="FECHA FIN" dataDxfId="28"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0100-000005000000}" name="ESTADO" dataDxfId="27"/>
+    <tableColumn id="1" name="TAREA"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="30"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="29"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="28"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="27"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF02000000}" name="Table134" displayName="Table134" ref="A2:E8" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A2:E8" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A2:E8" totalsRowShown="0" headerRowDxfId="23">
+  <autoFilter ref="A2:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0200-000001000000}" name="TAREA" dataDxfId="22"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0200-000002000000}" name="RESPONSABLE" dataDxfId="21"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0200-000003000000}" name="FECHA INICIO" dataDxfId="20"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0200-000004000000}" name="FECHA FIN" dataDxfId="19"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0200-000005000000}" name="ESTADO" dataDxfId="18"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="22"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="21"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="20"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="19"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="18"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{00000000-000C-0000-FFFF-FFFF03000000}" name="Table1345" displayName="Table1345" ref="A2:E11" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A2:E11" xr:uid="{00000000-0009-0000-0100-000004000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A2:E11" totalsRowShown="0" headerRowDxfId="14">
+  <autoFilter ref="A2:E11"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0300-000001000000}" name="TAREA" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0300-000002000000}" name="RESPONSABLE" dataDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0300-000003000000}" name="FECHA INICIO" dataDxfId="11"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0300-000004000000}" name="FECHA FIN" dataDxfId="10"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0300-000005000000}" name="ESTADO" dataDxfId="9"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="13"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="12"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="11"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="10"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{00000000-000C-0000-FFFF-FFFF04000000}" name="Table13456" displayName="Table13456" ref="A2:E9" totalsRowShown="0" headerRowDxfId="5">
-  <autoFilter ref="A2:E9" xr:uid="{00000000-0009-0000-0100-000005000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A2:E9" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A2:E9"/>
   <tableColumns count="5">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0400-000001000000}" name="TAREA" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0400-000002000000}" name="RESPONSABLE" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0400-000003000000}" name="FECHA INICIO" dataDxfId="2"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0400-000004000000}" name="FECHA FIN" dataDxfId="1"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0400-000005000000}" name="ESTADO" dataDxfId="0"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="4"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="3"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="2"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="1"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1375,28 +1374,28 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="96.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" customWidth="1"/>
+    <col min="1" max="1" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="51" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>62</v>
       </c>
       <c r="B1" s="32"/>
       <c r="C1" s="33"/>
     </row>
-    <row r="2" spans="1:3" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:3" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="19" t="s">
         <v>0</v>
       </c>
@@ -1407,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>1</v>
       </c>
@@ -1418,7 +1417,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>1</v>
       </c>
@@ -1427,7 +1426,7 @@
       </c>
       <c r="C4" s="29"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -1436,7 +1435,7 @@
       </c>
       <c r="C5" s="29"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>1</v>
       </c>
@@ -1445,7 +1444,7 @@
       </c>
       <c r="C6" s="29"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>1</v>
       </c>
@@ -1454,7 +1453,7 @@
       </c>
       <c r="C7" s="29"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>1</v>
       </c>
@@ -1463,7 +1462,7 @@
       </c>
       <c r="C8" s="29"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>1</v>
       </c>
@@ -1472,7 +1471,7 @@
       </c>
       <c r="C9" s="29"/>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>1</v>
       </c>
@@ -1481,7 +1480,7 @@
       </c>
       <c r="C10" s="30"/>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>2</v>
       </c>
@@ -1492,7 +1491,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="7">
         <v>2</v>
       </c>
@@ -1501,7 +1500,7 @@
       </c>
       <c r="C12" s="29"/>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>2</v>
       </c>
@@ -1510,7 +1509,7 @@
       </c>
       <c r="C13" s="29"/>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>2</v>
       </c>
@@ -1519,7 +1518,7 @@
       </c>
       <c r="C14" s="29"/>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>2</v>
       </c>
@@ -1528,7 +1527,7 @@
       </c>
       <c r="C15" s="29"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>2</v>
       </c>
@@ -1537,7 +1536,7 @@
       </c>
       <c r="C16" s="30"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="11">
         <v>3</v>
       </c>
@@ -1548,7 +1547,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>3</v>
       </c>
@@ -1557,7 +1556,7 @@
       </c>
       <c r="C18" s="29"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="10">
         <v>3</v>
       </c>
@@ -1566,7 +1565,7 @@
       </c>
       <c r="C19" s="29"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="10">
         <v>3</v>
       </c>
@@ -1575,7 +1574,7 @@
       </c>
       <c r="C20" s="29"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="10">
         <v>3</v>
       </c>
@@ -1584,7 +1583,7 @@
       </c>
       <c r="C21" s="29"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="14">
         <v>3</v>
       </c>
@@ -1593,7 +1592,7 @@
       </c>
       <c r="C22" s="30"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="17">
         <v>4</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="16">
         <v>4</v>
       </c>
@@ -1613,7 +1612,7 @@
       </c>
       <c r="C24" s="29"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="16">
         <v>4</v>
       </c>
@@ -1622,7 +1621,7 @@
       </c>
       <c r="C25" s="29"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="16">
         <v>4</v>
       </c>
@@ -1631,7 +1630,7 @@
       </c>
       <c r="C26" s="29"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="16">
         <v>4</v>
       </c>
@@ -1640,7 +1639,7 @@
       </c>
       <c r="C27" s="29"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="16">
         <v>4</v>
       </c>
@@ -1649,7 +1648,7 @@
       </c>
       <c r="C28" s="29"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="16">
         <v>4</v>
       </c>
@@ -1658,7 +1657,7 @@
       </c>
       <c r="C29" s="29"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="16">
         <v>4</v>
       </c>
@@ -1667,7 +1666,7 @@
       </c>
       <c r="C30" s="29"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="18">
         <v>4</v>
       </c>
@@ -1676,7 +1675,7 @@
       </c>
       <c r="C31" s="30"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="25">
         <v>5</v>
       </c>
@@ -1687,7 +1686,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="26">
         <v>5</v>
       </c>
@@ -1696,7 +1695,7 @@
       </c>
       <c r="C33" s="29"/>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="26">
         <v>5</v>
       </c>
@@ -1705,7 +1704,7 @@
       </c>
       <c r="C34" s="29"/>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="26">
         <v>5</v>
       </c>
@@ -1714,7 +1713,7 @@
       </c>
       <c r="C35" s="29"/>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="26">
         <v>5</v>
       </c>
@@ -1723,7 +1722,7 @@
       </c>
       <c r="C36" s="29"/>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="26">
         <v>5</v>
       </c>
@@ -1732,7 +1731,7 @@
       </c>
       <c r="C37" s="29"/>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="27">
         <v>5</v>
       </c>
@@ -1756,20 +1755,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>41</v>
       </c>
@@ -1778,7 +1777,7 @@
       <c r="D1" s="34"/>
       <c r="E1" s="34"/>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>42</v>
       </c>
@@ -1795,7 +1794,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
@@ -1812,7 +1811,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -1829,7 +1828,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>
@@ -1846,7 +1845,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
@@ -1863,7 +1862,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>7</v>
       </c>
@@ -1880,7 +1879,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1897,7 +1896,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1914,7 +1913,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>10</v>
       </c>
@@ -1949,7 +1948,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10" xr:uid="{00000000-0002-0000-0100-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E10">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1961,20 +1960,20 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="35" t="s">
         <v>56</v>
       </c>
@@ -1983,7 +1982,7 @@
       <c r="D1" s="35"/>
       <c r="E1" s="35"/>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>42</v>
       </c>
@@ -2000,7 +1999,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -2017,12 +2016,12 @@
         <v>55</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C4" s="22">
         <v>44445</v>
@@ -2031,10 +2030,10 @@
         <v>44457</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>14</v>
       </c>
@@ -2051,7 +2050,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>15</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>16</v>
       </c>
@@ -2085,12 +2084,12 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>17</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C8" s="22">
         <v>44445</v>
@@ -2120,7 +2119,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8" xr:uid="{00000000-0002-0000-0200-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2132,20 +2131,20 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="54.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="36" t="s">
         <v>59</v>
       </c>
@@ -2154,7 +2153,7 @@
       <c r="D1" s="36"/>
       <c r="E1" s="36"/>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>42</v>
       </c>
@@ -2171,7 +2170,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>19</v>
       </c>
@@ -2188,7 +2187,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>18</v>
       </c>
@@ -2205,7 +2204,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>20</v>
       </c>
@@ -2222,7 +2221,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>21</v>
       </c>
@@ -2239,7 +2238,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>28</v>
       </c>
@@ -2256,7 +2255,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="13" t="s">
         <v>22</v>
       </c>
@@ -2291,7 +2290,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2303,20 +2302,20 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="96.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="37" t="s">
         <v>60</v>
       </c>
@@ -2325,7 +2324,7 @@
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>42</v>
       </c>
@@ -2342,7 +2341,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>23</v>
       </c>
@@ -2359,7 +2358,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>24</v>
       </c>
@@ -2376,7 +2375,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>25</v>
       </c>
@@ -2393,7 +2392,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>26</v>
       </c>
@@ -2410,7 +2409,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>27</v>
       </c>
@@ -2427,7 +2426,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>29</v>
       </c>
@@ -2444,7 +2443,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>30</v>
       </c>
@@ -2461,7 +2460,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
         <v>31</v>
       </c>
@@ -2478,7 +2477,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
         <v>32</v>
       </c>
@@ -2513,7 +2512,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E11" xr:uid="{00000000-0002-0000-0400-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E11">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2525,20 +2524,20 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="96.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="5" width="20.6640625" customWidth="1"/>
+    <col min="1" max="1" width="96.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>61</v>
       </c>
@@ -2547,7 +2546,7 @@
       <c r="D1" s="38"/>
       <c r="E1" s="38"/>
     </row>
-    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="24" t="s">
         <v>42</v>
       </c>
@@ -2564,7 +2563,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="12" t="s">
         <v>35</v>
       </c>
@@ -2581,7 +2580,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
         <v>34</v>
       </c>
@@ -2598,7 +2597,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
         <v>36</v>
       </c>
@@ -2615,7 +2614,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
         <v>37</v>
       </c>
@@ -2632,7 +2631,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
         <v>38</v>
       </c>
@@ -2649,7 +2648,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
         <v>39</v>
       </c>
@@ -2666,7 +2665,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
         <v>40</v>
       </c>
@@ -2701,7 +2700,7 @@
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E9" xr:uid="{00000000-0002-0000-0500-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E9">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Actualizacion de produc Backlog
</commit_message>
<xml_diff>
--- a/Documentos Sprint/ProducBacklogDIVI.xlsx
+++ b/Documentos Sprint/ProducBacklogDIVI.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="2"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Backlog" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="69">
   <si>
     <t>SPRINT</t>
   </si>
@@ -218,6 +218,24 @@
   </si>
   <si>
     <t>PRODUCT BACKLOG - DIVI SAS</t>
+  </si>
+  <si>
+    <t>CREAR FORMULARIO DE INGRESO DE USUARIO HTML</t>
+  </si>
+  <si>
+    <t>ESTILIZAR FORMULARIO DE INGRESO DE USUARIOS EN CSS</t>
+  </si>
+  <si>
+    <t>MAYCOL - NICOLAS</t>
+  </si>
+  <si>
+    <t>GENERAR CÓDIGO EN JAVASCRIPT DEL FORMULARIO DE INGRESO DE USUARIO</t>
+  </si>
+  <si>
+    <t>PROGRAMAR CÓDIGO PARA GUARDAR INFORMACIÓN DE ACCESO A USUARIO EN LA BASE DE DATOS</t>
+  </si>
+  <si>
+    <t>PROGRAMAR CÓDIGO PARA GUARDAR INFORMACIÓN DE  USUARIO EN LA BASE DE DATOS</t>
   </si>
 </sst>
 </file>
@@ -581,7 +599,442 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="52">
+  <dxfs count="73">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00F8F2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF969696"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0066"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -618,42 +1071,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00F8F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF969696"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -689,45 +1106,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00F8F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF969696"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -760,42 +1138,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00F8F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF969696"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -823,42 +1165,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00F8F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF969696"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -886,42 +1192,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00F8F2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF969696"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0066"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border>
         <bottom style="thin">
           <color rgb="FFFF6600"/>
@@ -1002,19 +1272,19 @@
   </dxfs>
   <tableStyles count="3" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Table Style 1" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="51"/>
-      <tableStyleElement type="firstRowStripe" dxfId="50"/>
-      <tableStyleElement type="secondRowStripe" dxfId="49"/>
+      <tableStyleElement type="headerRow" dxfId="72"/>
+      <tableStyleElement type="firstRowStripe" dxfId="71"/>
+      <tableStyleElement type="secondRowStripe" dxfId="70"/>
     </tableStyle>
     <tableStyle name="Table Style 2" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="48"/>
-      <tableStyleElement type="firstRowStripe" dxfId="47"/>
-      <tableStyleElement type="secondRowStripe" dxfId="46"/>
+      <tableStyleElement type="headerRow" dxfId="69"/>
+      <tableStyleElement type="firstRowStripe" dxfId="68"/>
+      <tableStyleElement type="secondRowStripe" dxfId="67"/>
     </tableStyle>
     <tableStyle name="Table Style 3" pivot="0" count="3">
-      <tableStyleElement type="headerRow" dxfId="45"/>
-      <tableStyleElement type="firstRowStripe" dxfId="44"/>
-      <tableStyleElement type="secondRowStripe" dxfId="43"/>
+      <tableStyleElement type="headerRow" dxfId="66"/>
+      <tableStyleElement type="firstRowStripe" dxfId="65"/>
+      <tableStyleElement type="secondRowStripe" dxfId="64"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1043,70 +1313,70 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="39">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A2:E10" totalsRowShown="0" headerRowDxfId="63">
   <autoFilter ref="A2:E10"/>
   <tableColumns count="5">
     <tableColumn id="1" name="TAREA"/>
-    <tableColumn id="2" name="RESPONSABLE" dataDxfId="38"/>
-    <tableColumn id="3" name="FECHA INICIO" dataDxfId="37"/>
-    <tableColumn id="4" name="FECHA FIN" dataDxfId="36"/>
-    <tableColumn id="5" name="ESTADO" dataDxfId="35"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="62"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="61"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="60"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="59"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight12" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:E8" totalsRowShown="0" headerRowDxfId="31">
-  <autoFilter ref="A2:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table13" displayName="Table13" ref="A2:E9" totalsRowShown="0" headerRowDxfId="58">
+  <autoFilter ref="A2:E9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="TAREA"/>
-    <tableColumn id="2" name="RESPONSABLE" dataDxfId="30"/>
-    <tableColumn id="3" name="FECHA INICIO" dataDxfId="29"/>
-    <tableColumn id="4" name="FECHA FIN" dataDxfId="28"/>
-    <tableColumn id="5" name="ESTADO" dataDxfId="27"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="57"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="56"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="55"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="54"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A2:E8" totalsRowShown="0" headerRowDxfId="23">
-  <autoFilter ref="A2:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table134" displayName="Table134" ref="A2:E9" totalsRowShown="0" headerRowDxfId="53">
+  <autoFilter ref="A2:E9"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="TAREA" dataDxfId="22"/>
-    <tableColumn id="2" name="RESPONSABLE" dataDxfId="21"/>
-    <tableColumn id="3" name="FECHA INICIO" dataDxfId="20"/>
-    <tableColumn id="4" name="FECHA FIN" dataDxfId="19"/>
-    <tableColumn id="5" name="ESTADO" dataDxfId="18"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="52"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="33"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="51"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="50"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="49"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A2:E11" totalsRowShown="0" headerRowDxfId="14">
-  <autoFilter ref="A2:E11"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1345" displayName="Table1345" ref="A2:E13" totalsRowShown="0" headerRowDxfId="48">
+  <autoFilter ref="A2:E13"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="TAREA" dataDxfId="13"/>
-    <tableColumn id="2" name="RESPONSABLE" dataDxfId="12"/>
-    <tableColumn id="3" name="FECHA INICIO" dataDxfId="11"/>
-    <tableColumn id="4" name="FECHA FIN" dataDxfId="10"/>
-    <tableColumn id="5" name="ESTADO" dataDxfId="9"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="47"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="46"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="45"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="44"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="43"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A2:E9" totalsRowShown="0" headerRowDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="5" name="Table13456" displayName="Table13456" ref="A2:E9" totalsRowShown="0" headerRowDxfId="42">
   <autoFilter ref="A2:E9"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="TAREA" dataDxfId="4"/>
-    <tableColumn id="2" name="RESPONSABLE" dataDxfId="3"/>
-    <tableColumn id="3" name="FECHA INICIO" dataDxfId="2"/>
-    <tableColumn id="4" name="FECHA FIN" dataDxfId="1"/>
-    <tableColumn id="5" name="ESTADO" dataDxfId="0"/>
+    <tableColumn id="1" name="TAREA" dataDxfId="41"/>
+    <tableColumn id="2" name="RESPONSABLE" dataDxfId="40"/>
+    <tableColumn id="3" name="FECHA INICIO" dataDxfId="39"/>
+    <tableColumn id="4" name="FECHA FIN" dataDxfId="38"/>
+    <tableColumn id="5" name="ESTADO" dataDxfId="37"/>
   </tableColumns>
   <tableStyleInfo name="Table Style 1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1935,15 +2205,15 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E10">
-    <cfRule type="containsText" dxfId="42" priority="2" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="3" operator="containsText" text="PENDIENTE">
+    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="PENDIENTE">
       <formula>NOT(ISERROR(SEARCH("PENDIENTE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E10">
-    <cfRule type="containsText" dxfId="40" priority="1" operator="containsText" text="TERMINADO">
+    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="TERMINADO">
       <formula>NOT(ISERROR(SEARCH("TERMINADO",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -1961,10 +2231,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2101,25 +2371,53 @@
         <v>53</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>63</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="22">
+        <v>44445</v>
+      </c>
+      <c r="D9" s="22">
+        <v>44457</v>
+      </c>
+      <c r="E9" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E8">
-    <cfRule type="containsText" dxfId="34" priority="2" operator="containsText" text="EN PROGRESO">
+  <conditionalFormatting sqref="E3:E9">
+    <cfRule type="containsText" dxfId="23" priority="5" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="33" priority="3" operator="containsText" text="PENDIENTE">
+    <cfRule type="containsText" dxfId="22" priority="6" operator="containsText" text="PENDIENTE">
       <formula>NOT(ISERROR(SEARCH("PENDIENTE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E8">
-    <cfRule type="containsText" dxfId="32" priority="1" operator="containsText" text="TERMINADO">
+  <conditionalFormatting sqref="E3:E9">
+    <cfRule type="containsText" dxfId="21" priority="4" operator="containsText" text="TERMINADO">
       <formula>NOT(ISERROR(SEARCH("TERMINADO",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="20" priority="2" operator="containsText" text="EN PROGRESO">
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="3" operator="containsText" text="PENDIENTE">
+      <formula>NOT(ISERROR(SEARCH("PENDIENTE",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="18" priority="1" operator="containsText" text="TERMINADO">
+      <formula>NOT(ISERROR(SEARCH("TERMINADO",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E9">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2132,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2175,7 +2473,7 @@
         <v>19</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="22">
         <v>44452</v>
@@ -2184,7 +2482,7 @@
         <v>44457</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2201,7 +2499,7 @@
         <v>44457</v>
       </c>
       <c r="E4" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2218,7 +2516,7 @@
         <v>44457</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2235,7 +2533,7 @@
         <v>44457</v>
       </c>
       <c r="E6" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2243,7 +2541,7 @@
         <v>28</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" s="22">
         <v>44452</v>
@@ -2252,16 +2550,14 @@
         <v>44457</v>
       </c>
       <c r="E7" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>48</v>
-      </c>
+      <c r="A8" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="22">
         <v>44452</v>
       </c>
@@ -2269,6 +2565,21 @@
         <v>44460</v>
       </c>
       <c r="E8" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" s="15"/>
+      <c r="C9" s="22">
+        <v>44452</v>
+      </c>
+      <c r="D9" s="22">
+        <v>44460</v>
+      </c>
+      <c r="E9" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2277,20 +2588,33 @@
     <mergeCell ref="A1:E1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E8">
-    <cfRule type="containsText" dxfId="26" priority="2" operator="containsText" text="EN PROGRESO">
+    <cfRule type="containsText" dxfId="17" priority="5" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="3" operator="containsText" text="PENDIENTE">
+    <cfRule type="containsText" dxfId="16" priority="6" operator="containsText" text="PENDIENTE">
       <formula>NOT(ISERROR(SEARCH("PENDIENTE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3:E8">
-    <cfRule type="containsText" dxfId="24" priority="1" operator="containsText" text="TERMINADO">
+    <cfRule type="containsText" dxfId="15" priority="4" operator="containsText" text="TERMINADO">
       <formula>NOT(ISERROR(SEARCH("TERMINADO",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="14" priority="2" operator="containsText" text="EN PROGRESO">
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="13" priority="3" operator="containsText" text="PENDIENTE">
+      <formula>NOT(ISERROR(SEARCH("PENDIENTE",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="TERMINADO">
+      <formula>NOT(ISERROR(SEARCH("TERMINADO",E9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E9">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2303,10 +2627,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2346,7 +2670,7 @@
         <v>23</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C3" s="22">
         <v>44459</v>
@@ -2355,7 +2679,7 @@
         <v>44466</v>
       </c>
       <c r="E3" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2389,7 +2713,7 @@
         <v>44466</v>
       </c>
       <c r="E5" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2414,7 +2738,7 @@
         <v>27</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="C7" s="22">
         <v>44459</v>
@@ -2427,28 +2751,26 @@
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B8" s="15" t="s">
-        <v>57</v>
-      </c>
+      <c r="A8" s="12" t="s">
+        <v>66</v>
+      </c>
+      <c r="B8" s="15"/>
       <c r="C8" s="22">
+        <v>44459</v>
+      </c>
+      <c r="D8" s="22">
         <v>44466</v>
       </c>
-      <c r="D8" s="22">
-        <v>44471</v>
-      </c>
       <c r="E8" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>30</v>
+        <v>67</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="C9" s="22">
         <v>44466</v>
@@ -2462,10 +2784,10 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B10" s="15" t="s">
-        <v>48</v>
+        <v>57</v>
       </c>
       <c r="C10" s="22">
         <v>44466</v>
@@ -2479,10 +2801,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" s="15" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="C11" s="22">
         <v>44466</v>
@@ -2491,6 +2813,38 @@
         <v>44471</v>
       </c>
       <c r="E11" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="15" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="22">
+        <v>44466</v>
+      </c>
+      <c r="D12" s="22">
+        <v>44471</v>
+      </c>
+      <c r="E12" s="23" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B13" s="15"/>
+      <c r="C13" s="22">
+        <v>44466</v>
+      </c>
+      <c r="D13" s="22">
+        <v>44471</v>
+      </c>
+      <c r="E13" s="23" t="s">
         <v>54</v>
       </c>
     </row>
@@ -2498,21 +2852,47 @@
   <mergeCells count="1">
     <mergeCell ref="A1:E1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E11">
-    <cfRule type="containsText" dxfId="17" priority="2" operator="containsText" text="EN PROGRESO">
+  <conditionalFormatting sqref="E3:E7 E9:E12">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="EN PROGRESO">
       <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E3)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="16" priority="3" operator="containsText" text="PENDIENTE">
+    <cfRule type="containsText" dxfId="10" priority="9" operator="containsText" text="PENDIENTE">
       <formula>NOT(ISERROR(SEARCH("PENDIENTE",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E11">
-    <cfRule type="containsText" dxfId="15" priority="1" operator="containsText" text="TERMINADO">
+  <conditionalFormatting sqref="E3:E7 E9:E12">
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="TERMINADO">
       <formula>NOT(ISERROR(SEARCH("TERMINADO",E3)))</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="5" priority="5" operator="containsText" text="EN PROGRESO">
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="4" priority="6" operator="containsText" text="PENDIENTE">
+      <formula>NOT(ISERROR(SEARCH("PENDIENTE",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="TERMINADO">
+      <formula>NOT(ISERROR(SEARCH("TERMINADO",E8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="2" priority="2" operator="containsText" text="EN PROGRESO">
+      <formula>NOT(ISERROR(SEARCH("EN PROGRESO",E13)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="PENDIENTE">
+      <formula>NOT(ISERROR(SEARCH("PENDIENTE",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="TERMINADO">
+      <formula>NOT(ISERROR(SEARCH("TERMINADO",E13)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E11">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E3:E13">
       <formula1>"PENDIENTE, EN PROGRESO, TERMINADO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>